<commit_message>
Slutgiltig v02, ej granskad
</commit_message>
<xml_diff>
--- a/DOKUMENT/TIDPLANERING/tidplan_v0.2.xlsx
+++ b/DOKUMENT/TIDPLANERING/tidplan_v0.2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basplan" sheetId="1" r:id="rId1"/>
@@ -1322,15 +1322,129 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1339,26 +1453,15 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1370,130 +1473,85 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1545,64 +1603,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1918,7 +1918,7 @@
   </sheetPr>
   <dimension ref="A1:AF60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B53" sqref="B53:D53"/>
     </sheetView>
   </sheetViews>
@@ -1938,211 +1938,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="146"/>
-      <c r="S1" s="146"/>
-      <c r="T1" s="146"/>
-      <c r="U1" s="146"/>
-      <c r="V1" s="146"/>
-      <c r="W1" s="146"/>
-      <c r="X1" s="146"/>
-      <c r="Y1" s="146"/>
-      <c r="Z1" s="146"/>
-      <c r="AA1" s="146"/>
-      <c r="AB1" s="146"/>
-      <c r="AC1" s="146"/>
-      <c r="AD1" s="146"/>
-      <c r="AE1" s="147"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="106"/>
     </row>
     <row r="2" spans="1:32" s="3" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="125"/>
+      <c r="B2" s="151"/>
       <c r="C2" s="24"/>
-      <c r="D2" s="148" t="s">
+      <c r="D2" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
-      <c r="N2" s="148"/>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="S2" s="148"/>
-      <c r="T2" s="148"/>
-      <c r="U2" s="148"/>
-      <c r="V2" s="148"/>
-      <c r="W2" s="148"/>
-      <c r="X2" s="148"/>
-      <c r="Y2" s="148"/>
-      <c r="Z2" s="148"/>
-      <c r="AA2" s="148"/>
-      <c r="AB2" s="148"/>
-      <c r="AC2" s="148"/>
-      <c r="AD2" s="148"/>
-      <c r="AE2" s="149"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
+      <c r="N2" s="107"/>
+      <c r="O2" s="107"/>
+      <c r="P2" s="107"/>
+      <c r="Q2" s="107"/>
+      <c r="R2" s="107"/>
+      <c r="S2" s="107"/>
+      <c r="T2" s="107"/>
+      <c r="U2" s="107"/>
+      <c r="V2" s="107"/>
+      <c r="W2" s="107"/>
+      <c r="X2" s="107"/>
+      <c r="Y2" s="107"/>
+      <c r="Z2" s="107"/>
+      <c r="AA2" s="107"/>
+      <c r="AB2" s="107"/>
+      <c r="AC2" s="107"/>
+      <c r="AD2" s="107"/>
+      <c r="AE2" s="108"/>
     </row>
     <row r="3" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="123"/>
+      <c r="B3" s="138"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="137">
+      <c r="D3" s="129">
         <v>2</v>
       </c>
-      <c r="E3" s="137"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="122" t="s">
+      <c r="E3" s="129"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="154">
+      <c r="H3" s="138"/>
+      <c r="I3" s="121">
         <v>42051</v>
       </c>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="154"/>
-      <c r="M3" s="154"/>
-      <c r="N3" s="154"/>
-      <c r="O3" s="155"/>
-      <c r="P3" s="122" t="s">
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="121"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="123"/>
-      <c r="R3" s="123"/>
-      <c r="S3" s="123"/>
-      <c r="T3" s="123"/>
-      <c r="U3" s="116"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="116"/>
-      <c r="X3" s="116"/>
-      <c r="Y3" s="116"/>
-      <c r="Z3" s="116"/>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="116"/>
-      <c r="AC3" s="116"/>
-      <c r="AD3" s="116"/>
-      <c r="AE3" s="117"/>
+      <c r="Q3" s="138"/>
+      <c r="R3" s="138"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="138"/>
+      <c r="U3" s="144"/>
+      <c r="V3" s="144"/>
+      <c r="W3" s="144"/>
+      <c r="X3" s="144"/>
+      <c r="Y3" s="144"/>
+      <c r="Z3" s="144"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="144"/>
+      <c r="AC3" s="144"/>
+      <c r="AD3" s="144"/>
+      <c r="AE3" s="145"/>
     </row>
     <row r="4" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="128" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="129"/>
+      <c r="A4" s="135" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="136"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="139"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="128" t="s">
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="129"/>
-      <c r="I4" s="156">
+      <c r="H4" s="136"/>
+      <c r="I4" s="123">
         <v>2</v>
       </c>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
-      <c r="O4" s="157"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="124"/>
       <c r="P4" s="26"/>
-      <c r="Q4" s="121" t="s">
+      <c r="Q4" s="149" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="121"/>
-      <c r="S4" s="121"/>
-      <c r="T4" s="121"/>
-      <c r="U4" s="121"/>
-      <c r="V4" s="121"/>
-      <c r="W4" s="121"/>
-      <c r="X4" s="121"/>
-      <c r="Y4" s="121"/>
-      <c r="Z4" s="121"/>
-      <c r="AA4" s="121"/>
-      <c r="AB4" s="121"/>
-      <c r="AC4" s="121"/>
-      <c r="AD4" s="121"/>
+      <c r="R4" s="149"/>
+      <c r="S4" s="149"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="149"/>
+      <c r="V4" s="149"/>
+      <c r="W4" s="149"/>
+      <c r="X4" s="149"/>
+      <c r="Y4" s="149"/>
+      <c r="Z4" s="149"/>
+      <c r="AA4" s="149"/>
+      <c r="AB4" s="149"/>
+      <c r="AC4" s="149"/>
+      <c r="AD4" s="149"/>
       <c r="AE4" s="27"/>
     </row>
     <row r="5" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="131"/>
+      <c r="B5" s="134"/>
       <c r="C5" s="28"/>
-      <c r="D5" s="141" t="s">
+      <c r="D5" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="141"/>
-      <c r="F5" s="142"/>
-      <c r="G5" s="130" t="s">
+      <c r="E5" s="125"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="131"/>
-      <c r="I5" s="141" t="s">
+      <c r="H5" s="134"/>
+      <c r="I5" s="125" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="141"/>
-      <c r="K5" s="141"/>
-      <c r="L5" s="141"/>
-      <c r="M5" s="141"/>
-      <c r="N5" s="141"/>
-      <c r="O5" s="142"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119"/>
-      <c r="W5" s="119"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="119"/>
-      <c r="Z5" s="119"/>
-      <c r="AA5" s="119"/>
-      <c r="AB5" s="119"/>
-      <c r="AC5" s="119"/>
-      <c r="AD5" s="119"/>
-      <c r="AE5" s="120"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="146"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="147"/>
+      <c r="AE5" s="148"/>
     </row>
     <row r="6" spans="1:32" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
       <c r="E6" s="42"/>
       <c r="F6" s="43" t="s">
         <v>12</v>
@@ -2150,42 +2150,42 @@
       <c r="G6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="126" t="s">
+      <c r="H6" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
-      <c r="T6" s="127"/>
-      <c r="U6" s="127"/>
-      <c r="V6" s="127"/>
-      <c r="W6" s="127"/>
-      <c r="X6" s="127"/>
-      <c r="Y6" s="127"/>
-      <c r="Z6" s="127"/>
-      <c r="AA6" s="127"/>
-      <c r="AB6" s="127"/>
-      <c r="AC6" s="127"/>
-      <c r="AD6" s="127"/>
-      <c r="AE6" s="150"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="110"/>
+      <c r="Q6" s="110"/>
+      <c r="R6" s="110"/>
+      <c r="S6" s="110"/>
+      <c r="T6" s="110"/>
+      <c r="U6" s="110"/>
+      <c r="V6" s="110"/>
+      <c r="W6" s="110"/>
+      <c r="X6" s="110"/>
+      <c r="Y6" s="110"/>
+      <c r="Z6" s="110"/>
+      <c r="AA6" s="110"/>
+      <c r="AB6" s="110"/>
+      <c r="AC6" s="110"/>
+      <c r="AD6" s="110"/>
+      <c r="AE6" s="111"/>
     </row>
     <row r="7" spans="1:32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="152"/>
-      <c r="D7" s="153"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="117"/>
       <c r="E7" s="30"/>
       <c r="F7" s="31" t="s">
         <v>13</v>
@@ -2270,11 +2270,11 @@
       <c r="A8" s="34">
         <v>1</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="134"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="143"/>
       <c r="E8" s="4"/>
       <c r="F8" s="58">
         <v>30</v>
@@ -2320,11 +2320,11 @@
       <c r="A9" s="35">
         <v>2</v>
       </c>
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="110"/>
-      <c r="D9" s="111"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="114"/>
       <c r="E9" s="4"/>
       <c r="F9" s="58">
         <v>5</v>
@@ -2366,11 +2366,11 @@
       <c r="A10" s="35">
         <v>3</v>
       </c>
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="111"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="114"/>
       <c r="E10" s="4"/>
       <c r="F10" s="58">
         <v>15</v>
@@ -2414,11 +2414,11 @@
       <c r="A11" s="36">
         <v>4</v>
       </c>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="106"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="119"/>
       <c r="E11" s="4"/>
       <c r="F11" s="58">
         <v>80</v>
@@ -2515,11 +2515,11 @@
       <c r="A13" s="97">
         <v>6</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="106"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="119"/>
       <c r="E13" s="4"/>
       <c r="F13" s="58">
         <v>70</v>
@@ -2563,11 +2563,11 @@
       <c r="A14" s="97">
         <v>7</v>
       </c>
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="106"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="119"/>
       <c r="E14" s="4"/>
       <c r="F14" s="58">
         <v>30</v>
@@ -2611,11 +2611,11 @@
       <c r="A15" s="97">
         <v>8</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="106"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="119"/>
       <c r="E15" s="4"/>
       <c r="F15" s="58">
         <v>70</v>
@@ -2659,11 +2659,11 @@
       <c r="A16" s="97">
         <v>9</v>
       </c>
-      <c r="B16" s="105" t="s">
+      <c r="B16" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="106"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="119"/>
       <c r="E16" s="4"/>
       <c r="F16" s="58">
         <v>40</v>
@@ -2707,11 +2707,11 @@
       <c r="A17" s="97">
         <v>10</v>
       </c>
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="106"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="119"/>
       <c r="E17" s="4"/>
       <c r="F17" s="58">
         <v>80</v>
@@ -2807,11 +2807,11 @@
       <c r="A19" s="97">
         <v>12</v>
       </c>
-      <c r="B19" s="144" t="s">
+      <c r="B19" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="114"/>
       <c r="E19" s="4"/>
       <c r="F19" s="58">
         <v>50</v>
@@ -2855,11 +2855,11 @@
       <c r="A20" s="97">
         <v>13</v>
       </c>
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="106"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="119"/>
       <c r="E20" s="4"/>
       <c r="F20" s="58">
         <v>20</v>
@@ -2901,11 +2901,11 @@
       <c r="A21" s="97">
         <v>14</v>
       </c>
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="106"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="119"/>
       <c r="E21" s="4"/>
       <c r="F21" s="58">
         <v>100</v>
@@ -2959,11 +2959,11 @@
       <c r="A22" s="97">
         <v>15</v>
       </c>
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="106"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="119"/>
       <c r="E22" s="4"/>
       <c r="F22" s="58">
         <v>100</v>
@@ -3009,11 +3009,11 @@
       <c r="A23" s="97">
         <v>16</v>
       </c>
-      <c r="B23" s="105" t="s">
+      <c r="B23" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="119"/>
       <c r="E23" s="4"/>
       <c r="F23" s="57">
         <v>20</v>
@@ -3055,11 +3055,11 @@
       <c r="A24" s="97">
         <v>17</v>
       </c>
-      <c r="B24" s="105" t="s">
+      <c r="B24" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="106"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="119"/>
       <c r="E24" s="7"/>
       <c r="F24" s="58">
         <v>100</v>
@@ -3113,11 +3113,11 @@
       <c r="A25" s="98">
         <v>18</v>
       </c>
-      <c r="B25" s="105" t="s">
+      <c r="B25" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="105"/>
-      <c r="D25" s="106"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="119"/>
       <c r="E25" s="4"/>
       <c r="F25" s="8">
         <v>100</v>
@@ -3160,11 +3160,11 @@
       <c r="A26" s="98">
         <v>19</v>
       </c>
-      <c r="B26" s="104" t="s">
+      <c r="B26" s="156" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="156"/>
       <c r="E26" s="4"/>
       <c r="F26" s="57">
         <v>200</v>
@@ -3204,11 +3204,11 @@
       <c r="A27" s="97">
         <v>20</v>
       </c>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="156" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
       <c r="E27" s="4"/>
       <c r="F27" s="8">
         <v>50</v>
@@ -3262,11 +3262,11 @@
       <c r="A28" s="97">
         <v>21</v>
       </c>
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="104"/>
-      <c r="D28" s="104"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
       <c r="E28" s="4"/>
       <c r="F28" s="8">
         <v>50</v>
@@ -3368,11 +3368,11 @@
       <c r="A30" s="97">
         <v>23</v>
       </c>
-      <c r="B30" s="104" t="s">
+      <c r="B30" s="156" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
+      <c r="C30" s="156"/>
+      <c r="D30" s="156"/>
       <c r="E30" s="4"/>
       <c r="F30" s="8">
         <v>25</v>
@@ -3418,11 +3418,11 @@
       <c r="A31" s="97">
         <v>24</v>
       </c>
-      <c r="B31" s="104" t="s">
+      <c r="B31" s="156" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="104"/>
-      <c r="D31" s="104"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="156"/>
       <c r="E31" s="4"/>
       <c r="F31" s="8">
         <v>25</v>
@@ -3468,11 +3468,11 @@
       <c r="A32" s="97">
         <v>25</v>
       </c>
-      <c r="B32" s="104" t="s">
+      <c r="B32" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
+      <c r="C32" s="156"/>
+      <c r="D32" s="156"/>
       <c r="E32" s="4"/>
       <c r="F32" s="8">
         <v>10</v>
@@ -3516,11 +3516,11 @@
       <c r="A33" s="97">
         <v>26</v>
       </c>
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="156" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="104"/>
-      <c r="D33" s="104"/>
+      <c r="C33" s="156"/>
+      <c r="D33" s="156"/>
       <c r="E33" s="4"/>
       <c r="F33" s="8">
         <v>10</v>
@@ -3600,11 +3600,11 @@
       <c r="A35" s="97">
         <v>28</v>
       </c>
-      <c r="B35" s="104" t="s">
+      <c r="B35" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="109"/>
-      <c r="D35" s="109"/>
+      <c r="C35" s="157"/>
+      <c r="D35" s="157"/>
       <c r="E35" s="4"/>
       <c r="F35" s="8">
         <v>40</v>
@@ -3674,9 +3674,9 @@
       <c r="A36" s="97">
         <v>29</v>
       </c>
-      <c r="B36" s="107"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="108"/>
+      <c r="B36" s="139"/>
+      <c r="C36" s="139"/>
+      <c r="D36" s="140"/>
       <c r="E36" s="4"/>
       <c r="F36" s="58"/>
       <c r="G36" s="5"/>
@@ -3712,11 +3712,11 @@
       <c r="A37" s="97">
         <v>30</v>
       </c>
-      <c r="B37" s="105" t="s">
+      <c r="B37" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="110"/>
-      <c r="D37" s="111"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="114"/>
       <c r="E37" s="4"/>
       <c r="F37" s="58"/>
       <c r="G37" s="5"/>
@@ -3754,11 +3754,11 @@
       <c r="A38" s="97">
         <v>31</v>
       </c>
-      <c r="B38" s="112" t="s">
+      <c r="B38" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="113"/>
-      <c r="D38" s="113"/>
+      <c r="C38" s="155"/>
+      <c r="D38" s="155"/>
       <c r="E38" s="4"/>
       <c r="F38" s="58"/>
       <c r="G38" s="5"/>
@@ -3796,11 +3796,11 @@
       <c r="A39" s="97">
         <v>32</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="110"/>
-      <c r="D39" s="111"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="114"/>
       <c r="E39" s="12"/>
       <c r="F39" s="9"/>
       <c r="G39" s="5"/>
@@ -3838,11 +3838,11 @@
       <c r="A40" s="97">
         <v>33</v>
       </c>
-      <c r="B40" s="112" t="s">
+      <c r="B40" s="154" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="113"/>
-      <c r="D40" s="113"/>
+      <c r="C40" s="155"/>
+      <c r="D40" s="155"/>
       <c r="E40" s="4"/>
       <c r="F40" s="58"/>
       <c r="G40" s="5"/>
@@ -3879,11 +3879,11 @@
       <c r="A41" s="97">
         <v>34</v>
       </c>
-      <c r="B41" s="105" t="s">
+      <c r="B41" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="110"/>
-      <c r="D41" s="111"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="114"/>
       <c r="E41" s="4"/>
       <c r="F41" s="63"/>
       <c r="G41" s="5"/>
@@ -3919,11 +3919,11 @@
       <c r="A42" s="97">
         <v>35</v>
       </c>
-      <c r="B42" s="112" t="s">
+      <c r="B42" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="113"/>
-      <c r="D42" s="113"/>
+      <c r="C42" s="155"/>
+      <c r="D42" s="155"/>
       <c r="E42" s="4"/>
       <c r="F42" s="58"/>
       <c r="G42" s="14"/>
@@ -3961,11 +3961,11 @@
       <c r="A43" s="97">
         <v>36</v>
       </c>
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="110"/>
-      <c r="D43" s="111"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="114"/>
       <c r="E43" s="4"/>
       <c r="F43" s="9"/>
       <c r="G43" s="73"/>
@@ -4003,9 +4003,9 @@
       <c r="A44" s="97">
         <v>37</v>
       </c>
-      <c r="B44" s="107"/>
-      <c r="C44" s="107"/>
-      <c r="D44" s="108"/>
+      <c r="B44" s="139"/>
+      <c r="C44" s="139"/>
+      <c r="D44" s="140"/>
       <c r="E44" s="4"/>
       <c r="F44" s="58"/>
       <c r="G44" s="73"/>
@@ -4041,11 +4041,11 @@
       <c r="A45" s="97">
         <v>38</v>
       </c>
-      <c r="B45" s="105" t="s">
+      <c r="B45" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="110"/>
-      <c r="D45" s="111"/>
+      <c r="C45" s="113"/>
+      <c r="D45" s="114"/>
       <c r="E45" s="4"/>
       <c r="F45" s="63"/>
       <c r="G45" s="73"/>
@@ -4081,11 +4081,11 @@
       <c r="A46" s="97">
         <v>39</v>
       </c>
-      <c r="B46" s="105" t="s">
+      <c r="B46" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="110"/>
-      <c r="D46" s="111"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="114"/>
       <c r="E46" s="4"/>
       <c r="F46" s="58"/>
       <c r="G46" s="73"/>
@@ -4121,11 +4121,11 @@
       <c r="A47" s="97">
         <v>40</v>
       </c>
-      <c r="B47" s="105" t="s">
+      <c r="B47" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="110"/>
-      <c r="D47" s="111"/>
+      <c r="C47" s="113"/>
+      <c r="D47" s="114"/>
       <c r="E47" s="4"/>
       <c r="F47" s="9"/>
       <c r="G47" s="73"/>
@@ -4161,11 +4161,11 @@
       <c r="A48" s="97">
         <v>41</v>
       </c>
-      <c r="B48" s="105" t="s">
+      <c r="B48" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="110"/>
-      <c r="D48" s="111"/>
+      <c r="C48" s="113"/>
+      <c r="D48" s="114"/>
       <c r="E48" s="4"/>
       <c r="F48" s="58"/>
       <c r="G48" s="73"/>
@@ -4201,11 +4201,11 @@
       <c r="A49" s="97">
         <v>42</v>
       </c>
-      <c r="B49" s="105" t="s">
+      <c r="B49" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="110"/>
-      <c r="D49" s="111"/>
+      <c r="C49" s="113"/>
+      <c r="D49" s="114"/>
       <c r="E49" s="4"/>
       <c r="F49" s="58"/>
       <c r="G49" s="73"/>
@@ -4241,11 +4241,11 @@
       <c r="A50" s="97">
         <v>43</v>
       </c>
-      <c r="B50" s="105" t="s">
+      <c r="B50" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="110"/>
-      <c r="D50" s="111"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="114"/>
       <c r="E50" s="4"/>
       <c r="F50" s="9"/>
       <c r="G50" s="73"/>
@@ -4281,11 +4281,11 @@
       <c r="A51" s="97">
         <v>44</v>
       </c>
-      <c r="B51" s="105" t="s">
+      <c r="B51" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="110"/>
-      <c r="D51" s="111"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="114"/>
       <c r="E51" s="4"/>
       <c r="F51" s="58"/>
       <c r="G51" s="73"/>
@@ -4321,11 +4321,11 @@
       <c r="A52" s="97">
         <v>45</v>
       </c>
-      <c r="B52" s="105" t="s">
+      <c r="B52" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="110"/>
-      <c r="D52" s="111"/>
+      <c r="C52" s="113"/>
+      <c r="D52" s="114"/>
       <c r="E52" s="4"/>
       <c r="F52" s="63"/>
       <c r="G52" s="73"/>
@@ -4361,11 +4361,11 @@
       <c r="A53" s="97">
         <v>46</v>
       </c>
-      <c r="B53" s="105" t="s">
+      <c r="B53" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="110"/>
-      <c r="D53" s="111"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="114"/>
       <c r="E53" s="4"/>
       <c r="F53" s="58"/>
       <c r="G53" s="73"/>
@@ -4401,11 +4401,11 @@
       <c r="A54" s="97">
         <v>47</v>
       </c>
-      <c r="B54" s="105" t="s">
+      <c r="B54" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="110"/>
-      <c r="D54" s="111"/>
+      <c r="C54" s="113"/>
+      <c r="D54" s="114"/>
       <c r="E54" s="4"/>
       <c r="F54" s="9"/>
       <c r="G54" s="73"/>
@@ -4440,11 +4440,11 @@
       <c r="A55" s="97">
         <v>48</v>
       </c>
-      <c r="B55" s="105" t="s">
+      <c r="B55" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="110"/>
-      <c r="D55" s="111"/>
+      <c r="C55" s="113"/>
+      <c r="D55" s="114"/>
       <c r="E55" s="4"/>
       <c r="F55" s="58"/>
       <c r="G55" s="73"/>
@@ -4480,11 +4480,11 @@
       <c r="A56" s="97">
         <v>49</v>
       </c>
-      <c r="B56" s="105" t="s">
+      <c r="B56" s="112" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="110"/>
-      <c r="D56" s="111"/>
+      <c r="C56" s="113"/>
+      <c r="D56" s="114"/>
       <c r="E56" s="4"/>
       <c r="F56" s="63"/>
       <c r="G56" s="73"/>
@@ -4519,9 +4519,9 @@
       <c r="A57" s="97">
         <v>50</v>
       </c>
-      <c r="B57" s="114"/>
-      <c r="C57" s="114"/>
-      <c r="D57" s="115"/>
+      <c r="B57" s="152"/>
+      <c r="C57" s="152"/>
+      <c r="D57" s="153"/>
       <c r="E57" s="4"/>
       <c r="F57" s="58"/>
       <c r="G57" s="74"/>
@@ -4557,9 +4557,9 @@
       <c r="A58" s="98">
         <v>51</v>
       </c>
-      <c r="B58" s="114"/>
-      <c r="C58" s="114"/>
-      <c r="D58" s="115"/>
+      <c r="B58" s="152"/>
+      <c r="C58" s="152"/>
+      <c r="D58" s="153"/>
       <c r="E58" s="4"/>
       <c r="F58" s="11"/>
       <c r="G58" s="12"/>
@@ -4593,11 +4593,11 @@
     </row>
     <row r="59" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="96"/>
-      <c r="B59" s="135" t="s">
+      <c r="B59" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="C59" s="135"/>
-      <c r="D59" s="136"/>
+      <c r="C59" s="127"/>
+      <c r="D59" s="128"/>
       <c r="E59" s="39"/>
       <c r="F59" s="40">
         <f>SUM(F8:F43)</f>
@@ -4775,20 +4775,44 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="70">
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="H6:AE6"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="U3:AE3"/>
+    <mergeCell ref="P5:AE5"/>
+    <mergeCell ref="Q4:AD4"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B59:D59"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="D4:F4"/>
@@ -4805,46 +4829,22 @@
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="H6:AE6"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="U3:AE3"/>
-    <mergeCell ref="P5:AE5"/>
-    <mergeCell ref="Q4:AD4"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -4860,8 +4860,8 @@
   </sheetPr>
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4876,240 +4876,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="177"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
+      <c r="W1" s="163"/>
+      <c r="X1" s="163"/>
+      <c r="Y1" s="163"/>
+      <c r="Z1" s="163"/>
+      <c r="AA1" s="163"/>
+      <c r="AB1" s="163"/>
+      <c r="AC1" s="163"/>
+      <c r="AD1" s="164"/>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="167" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="181"/>
+      <c r="B2" s="168"/>
       <c r="C2" s="45"/>
-      <c r="D2" s="178" t="str">
+      <c r="D2" s="165" t="str">
         <f>Basplan!D2</f>
         <v>Undsättningsrobot</v>
       </c>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="178"/>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178"/>
-      <c r="N2" s="178"/>
-      <c r="O2" s="178"/>
-      <c r="P2" s="178"/>
-      <c r="Q2" s="178"/>
-      <c r="R2" s="178"/>
-      <c r="S2" s="178"/>
-      <c r="T2" s="178"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="178"/>
-      <c r="W2" s="178"/>
-      <c r="X2" s="178"/>
-      <c r="Y2" s="178"/>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="178"/>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="179"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
+      <c r="U2" s="165"/>
+      <c r="V2" s="165"/>
+      <c r="W2" s="165"/>
+      <c r="X2" s="165"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="165"/>
+      <c r="AA2" s="165"/>
+      <c r="AB2" s="165"/>
+      <c r="AC2" s="165"/>
+      <c r="AD2" s="166"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="183"/>
+      <c r="B3" s="170"/>
       <c r="C3" s="46"/>
-      <c r="D3" s="184">
+      <c r="D3" s="171">
         <f>Basplan!D3</f>
         <v>2</v>
       </c>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="122" t="s">
+      <c r="E3" s="172"/>
+      <c r="F3" s="172"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="187"/>
-      <c r="L3" s="154">
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="121">
         <v>42051</v>
       </c>
-      <c r="M3" s="188"/>
-      <c r="N3" s="188"/>
-      <c r="O3" s="188"/>
-      <c r="P3" s="188"/>
-      <c r="Q3" s="188"/>
-      <c r="R3" s="188"/>
-      <c r="S3" s="188"/>
-      <c r="T3" s="188"/>
-      <c r="U3" s="188"/>
-      <c r="V3" s="188"/>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="188"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="188"/>
-      <c r="AB3" s="188"/>
-      <c r="AC3" s="188"/>
-      <c r="AD3" s="189"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="175"/>
+      <c r="S3" s="175"/>
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="175"/>
+      <c r="AA3" s="175"/>
+      <c r="AB3" s="175"/>
+      <c r="AC3" s="175"/>
+      <c r="AD3" s="176"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="159" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="169"/>
+      <c r="A4" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="188"/>
       <c r="C4" s="47"/>
-      <c r="D4" s="170" t="str">
+      <c r="D4" s="189" t="str">
         <f>Basplan!D4</f>
         <v>Kent Palmkvist</v>
       </c>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="172"/>
-      <c r="H4" s="159" t="s">
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="160"/>
-      <c r="J4" s="160"/>
-      <c r="K4" s="160"/>
-      <c r="L4" s="161" t="s">
+      <c r="I4" s="179"/>
+      <c r="J4" s="179"/>
+      <c r="K4" s="179"/>
+      <c r="L4" s="180" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="162"/>
-      <c r="N4" s="162"/>
-      <c r="O4" s="162"/>
-      <c r="P4" s="162"/>
-      <c r="Q4" s="162"/>
-      <c r="R4" s="162"/>
-      <c r="S4" s="162"/>
-      <c r="T4" s="162"/>
-      <c r="U4" s="162"/>
-      <c r="V4" s="162"/>
-      <c r="W4" s="162"/>
-      <c r="X4" s="162"/>
-      <c r="Y4" s="162"/>
-      <c r="Z4" s="162"/>
-      <c r="AA4" s="162"/>
-      <c r="AB4" s="162"/>
-      <c r="AC4" s="162"/>
-      <c r="AD4" s="163"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="181"/>
+      <c r="O4" s="181"/>
+      <c r="P4" s="181"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="181"/>
+      <c r="S4" s="181"/>
+      <c r="T4" s="181"/>
+      <c r="U4" s="181"/>
+      <c r="V4" s="181"/>
+      <c r="W4" s="181"/>
+      <c r="X4" s="181"/>
+      <c r="Y4" s="181"/>
+      <c r="Z4" s="181"/>
+      <c r="AA4" s="181"/>
+      <c r="AB4" s="181"/>
+      <c r="AC4" s="181"/>
+      <c r="AD4" s="182"/>
     </row>
     <row r="5" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="192" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="193"/>
       <c r="C5" s="48"/>
-      <c r="D5" s="190" t="str">
+      <c r="D5" s="159" t="str">
         <f>Basplan!D5</f>
         <v>TSEA56</v>
       </c>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="192"/>
-      <c r="H5" s="158"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="119"/>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119"/>
-      <c r="W5" s="119"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="119"/>
-      <c r="Z5" s="119"/>
-      <c r="AA5" s="119"/>
-      <c r="AB5" s="119"/>
-      <c r="AC5" s="119"/>
-      <c r="AD5" s="120"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="148"/>
     </row>
     <row r="6" spans="1:31" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="167" t="s">
+      <c r="A6" s="186" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="168"/>
-      <c r="C6" s="168"/>
-      <c r="D6" s="168"/>
-      <c r="E6" s="168"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="164" t="s">
+      <c r="B6" s="187"/>
+      <c r="C6" s="187"/>
+      <c r="D6" s="187"/>
+      <c r="E6" s="187"/>
+      <c r="F6" s="187"/>
+      <c r="G6" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="165"/>
-      <c r="I6" s="165"/>
-      <c r="J6" s="165"/>
-      <c r="K6" s="165"/>
-      <c r="L6" s="165"/>
-      <c r="M6" s="165"/>
-      <c r="N6" s="165"/>
-      <c r="O6" s="165"/>
-      <c r="P6" s="165"/>
-      <c r="Q6" s="165"/>
-      <c r="R6" s="165"/>
-      <c r="S6" s="165"/>
-      <c r="T6" s="165"/>
-      <c r="U6" s="165"/>
-      <c r="V6" s="165"/>
-      <c r="W6" s="165"/>
-      <c r="X6" s="165"/>
-      <c r="Y6" s="165"/>
-      <c r="Z6" s="165"/>
-      <c r="AA6" s="165"/>
-      <c r="AB6" s="165"/>
-      <c r="AC6" s="165"/>
-      <c r="AD6" s="166"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="184"/>
+      <c r="L6" s="184"/>
+      <c r="M6" s="184"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="184"/>
+      <c r="P6" s="184"/>
+      <c r="Q6" s="184"/>
+      <c r="R6" s="184"/>
+      <c r="S6" s="184"/>
+      <c r="T6" s="184"/>
+      <c r="U6" s="184"/>
+      <c r="V6" s="184"/>
+      <c r="W6" s="184"/>
+      <c r="X6" s="184"/>
+      <c r="Y6" s="184"/>
+      <c r="Z6" s="184"/>
+      <c r="AA6" s="184"/>
+      <c r="AB6" s="184"/>
+      <c r="AC6" s="184"/>
+      <c r="AD6" s="185"/>
     </row>
     <row r="7" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="152"/>
-      <c r="D7" s="152"/>
-      <c r="E7" s="152"/>
-      <c r="F7" s="152"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
       <c r="G7" s="31">
         <f>Basplan!H7</f>
         <v>1</v>
@@ -5208,13 +5208,13 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="141" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="134"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="143"/>
       <c r="G8" s="66"/>
       <c r="H8" s="67"/>
       <c r="I8" s="67"/>
@@ -5251,13 +5251,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="110"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="68"/>
       <c r="H9" s="69"/>
       <c r="I9" s="69"/>
@@ -5294,13 +5294,13 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="110"/>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="111"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="114"/>
       <c r="G10" s="68"/>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
@@ -5337,13 +5337,13 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
-      <c r="B11" s="144" t="s">
+      <c r="B11" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="111"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="114"/>
       <c r="G11" s="68"/>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
@@ -5380,13 +5380,13 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="54"/>
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="111"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="114"/>
       <c r="G12" s="68"/>
       <c r="H12" s="69"/>
       <c r="I12" s="69"/>
@@ -5424,13 +5424,13 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
-      <c r="B13" s="144" t="s">
+      <c r="B13" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
       <c r="G13" s="68"/>
       <c r="H13" s="69"/>
       <c r="I13" s="69"/>
@@ -5442,7 +5442,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="19">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
@@ -5462,16 +5462,16 @@
       <c r="AC13" s="20"/>
       <c r="AD13" s="52">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
-      <c r="B14" s="144"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -5502,11 +5502,11 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
-      <c r="B15" s="144"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
@@ -5537,11 +5537,11 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
-      <c r="B16" s="144"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -5572,11 +5572,11 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
-      <c r="B17" s="144"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -5607,11 +5607,11 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
-      <c r="B18" s="144"/>
-      <c r="C18" s="110"/>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -5642,11 +5642,11 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
-      <c r="B19" s="144"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
@@ -5677,11 +5677,11 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
-      <c r="B20" s="144"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="113"/>
       <c r="G20" s="18"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -5712,11 +5712,11 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
-      <c r="B21" s="144"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -5747,11 +5747,11 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
-      <c r="B22" s="144"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
@@ -5782,11 +5782,11 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="54"/>
-      <c r="B23" s="144"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
       <c r="G23" s="18"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -5817,11 +5817,11 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="54"/>
-      <c r="B24" s="144"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
       <c r="G24" s="18"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
@@ -5852,11 +5852,11 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
-      <c r="B25" s="144"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="110"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
       <c r="G25" s="18"/>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
@@ -5887,11 +5887,11 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
-      <c r="B26" s="144"/>
-      <c r="C26" s="110"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="110"/>
+      <c r="B26" s="120"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
       <c r="G26" s="18"/>
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
@@ -5922,11 +5922,11 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
       <c r="G27" s="18"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
@@ -5957,11 +5957,11 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="55"/>
-      <c r="B28" s="144"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
       <c r="G28" s="18"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
@@ -5992,11 +5992,11 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="55"/>
-      <c r="B29" s="144"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
@@ -6027,11 +6027,11 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="54"/>
-      <c r="B30" s="144"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="110"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="113"/>
       <c r="G30" s="18"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
@@ -6062,11 +6062,11 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="54"/>
-      <c r="B31" s="144"/>
-      <c r="C31" s="110"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="110"/>
-      <c r="F31" s="110"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
       <c r="G31" s="18"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
@@ -6097,11 +6097,11 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="54"/>
-      <c r="B32" s="144"/>
-      <c r="C32" s="110"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
+      <c r="B32" s="120"/>
+      <c r="C32" s="113"/>
+      <c r="D32" s="113"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="113"/>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
@@ -6132,11 +6132,11 @@
     </row>
     <row r="33" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="54"/>
-      <c r="B33" s="193"/>
-      <c r="C33" s="114"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="114"/>
+      <c r="B33" s="158"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
       <c r="G33" s="21"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -6167,13 +6167,13 @@
     </row>
     <row r="34" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
-      <c r="B34" s="135" t="s">
+      <c r="B34" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="135"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
-      <c r="F34" s="135"/>
+      <c r="C34" s="127"/>
+      <c r="D34" s="127"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
       <c r="G34" s="56">
         <f>SUM(G8:G33)</f>
         <v>0</v>
@@ -6200,7 +6200,7 @@
       </c>
       <c r="M34" s="56">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="N34" s="56">
         <f t="shared" si="1"/>
@@ -6268,12 +6268,40 @@
       </c>
       <c r="AD34" s="53">
         <f>SUM(AD8:AD33)</f>
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="H5:AD5"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:AD4"/>
+    <mergeCell ref="G6:AD6"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="D2:AD2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:AD3"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B19:F19"/>
@@ -6290,34 +6318,6 @@
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="D2:AD2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:AD3"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="H5:AD5"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:AD4"/>
-    <mergeCell ref="G6:AD6"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.71" top="1" bottom="1" header="0.5" footer="0.61"/>

</xml_diff>

<commit_message>
korrigeringar i v0.2 av plan/systemskiss
</commit_message>
<xml_diff>
--- a/DOKUMENT/TIDPLANERING/tidplan_v0.2.xlsx
+++ b/DOKUMENT/TIDPLANERING/tidplan_v0.2.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Måns\Documents\GitHub\TSEA56Grupp2\DOKUMENT\TIDPLANERING\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Basplan" sheetId="1" r:id="rId1"/>
     <sheet name="Summering TID" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -301,6 +296,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -326,10 +322,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -346,6 +344,7 @@
     <font>
       <sz val="7"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1066,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1322,36 +1321,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1360,108 +1347,17 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1473,39 +1369,180 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1553,56 +1590,21 @@
     <xf numFmtId="14" fontId="5" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1669,7 +1671,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1704,7 +1706,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1918,8 +1920,8 @@
   </sheetPr>
   <dimension ref="A1:AF60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1938,211 +1940,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="106"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="144"/>
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="144"/>
+      <c r="R1" s="144"/>
+      <c r="S1" s="144"/>
+      <c r="T1" s="144"/>
+      <c r="U1" s="144"/>
+      <c r="V1" s="144"/>
+      <c r="W1" s="144"/>
+      <c r="X1" s="144"/>
+      <c r="Y1" s="144"/>
+      <c r="Z1" s="144"/>
+      <c r="AA1" s="144"/>
+      <c r="AB1" s="144"/>
+      <c r="AC1" s="144"/>
+      <c r="AD1" s="144"/>
+      <c r="AE1" s="145"/>
     </row>
     <row r="2" spans="1:32" s="3" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="151"/>
+      <c r="B2" s="125"/>
       <c r="C2" s="24"/>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="146" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="107"/>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="107"/>
-      <c r="AE2" s="108"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
+      <c r="O2" s="146"/>
+      <c r="P2" s="146"/>
+      <c r="Q2" s="146"/>
+      <c r="R2" s="146"/>
+      <c r="S2" s="146"/>
+      <c r="T2" s="146"/>
+      <c r="U2" s="146"/>
+      <c r="V2" s="146"/>
+      <c r="W2" s="146"/>
+      <c r="X2" s="146"/>
+      <c r="Y2" s="146"/>
+      <c r="Z2" s="146"/>
+      <c r="AA2" s="146"/>
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="146"/>
+      <c r="AD2" s="146"/>
+      <c r="AE2" s="147"/>
     </row>
     <row r="3" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="138"/>
+      <c r="B3" s="123"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="129">
+      <c r="D3" s="135">
         <v>2</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="137" t="s">
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="138"/>
-      <c r="I3" s="121">
-        <v>42051</v>
-      </c>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="137" t="s">
+      <c r="H3" s="123"/>
+      <c r="I3" s="154">
+        <v>42053</v>
+      </c>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
+      <c r="M3" s="154"/>
+      <c r="N3" s="154"/>
+      <c r="O3" s="155"/>
+      <c r="P3" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="138"/>
-      <c r="U3" s="144"/>
-      <c r="V3" s="144"/>
-      <c r="W3" s="144"/>
-      <c r="X3" s="144"/>
-      <c r="Y3" s="144"/>
-      <c r="Z3" s="144"/>
-      <c r="AA3" s="144"/>
-      <c r="AB3" s="144"/>
-      <c r="AC3" s="144"/>
-      <c r="AD3" s="144"/>
-      <c r="AE3" s="145"/>
+      <c r="Q3" s="123"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="123"/>
+      <c r="U3" s="116"/>
+      <c r="V3" s="116"/>
+      <c r="W3" s="116"/>
+      <c r="X3" s="116"/>
+      <c r="Y3" s="116"/>
+      <c r="Z3" s="116"/>
+      <c r="AA3" s="116"/>
+      <c r="AB3" s="116"/>
+      <c r="AC3" s="116"/>
+      <c r="AD3" s="116"/>
+      <c r="AE3" s="117"/>
     </row>
     <row r="4" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="135" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="136"/>
+      <c r="A4" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="127"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="131" t="s">
+      <c r="D4" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="135" t="s">
+      <c r="E4" s="137"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="136"/>
-      <c r="I4" s="123">
+      <c r="H4" s="127"/>
+      <c r="I4" s="156">
         <v>2</v>
       </c>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="123"/>
-      <c r="O4" s="124"/>
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="157"/>
       <c r="P4" s="26"/>
-      <c r="Q4" s="149" t="s">
+      <c r="Q4" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="149"/>
-      <c r="S4" s="149"/>
-      <c r="T4" s="149"/>
-      <c r="U4" s="149"/>
-      <c r="V4" s="149"/>
-      <c r="W4" s="149"/>
-      <c r="X4" s="149"/>
-      <c r="Y4" s="149"/>
-      <c r="Z4" s="149"/>
-      <c r="AA4" s="149"/>
-      <c r="AB4" s="149"/>
-      <c r="AC4" s="149"/>
-      <c r="AD4" s="149"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="121"/>
+      <c r="T4" s="121"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="121"/>
+      <c r="X4" s="121"/>
+      <c r="Y4" s="121"/>
+      <c r="Z4" s="121"/>
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="121"/>
+      <c r="AC4" s="121"/>
+      <c r="AD4" s="121"/>
       <c r="AE4" s="27"/>
     </row>
     <row r="5" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="133" t="s">
+      <c r="A5" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="134"/>
+      <c r="B5" s="129"/>
       <c r="C5" s="28"/>
-      <c r="D5" s="125" t="s">
+      <c r="D5" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="133" t="s">
+      <c r="E5" s="139"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="134"/>
-      <c r="I5" s="125" t="s">
+      <c r="H5" s="129"/>
+      <c r="I5" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
-      <c r="O5" s="126"/>
-      <c r="P5" s="146"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147"/>
-      <c r="AE5" s="148"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="139"/>
+      <c r="M5" s="139"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119"/>
+      <c r="T5" s="119"/>
+      <c r="U5" s="119"/>
+      <c r="V5" s="119"/>
+      <c r="W5" s="119"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="119"/>
+      <c r="Z5" s="119"/>
+      <c r="AA5" s="119"/>
+      <c r="AB5" s="119"/>
+      <c r="AC5" s="119"/>
+      <c r="AD5" s="119"/>
+      <c r="AE5" s="120"/>
     </row>
     <row r="6" spans="1:32" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
+      <c r="B6" s="149"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
       <c r="E6" s="42"/>
       <c r="F6" s="43" t="s">
         <v>12</v>
@@ -2150,42 +2152,42 @@
       <c r="G6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
-      <c r="S6" s="110"/>
-      <c r="T6" s="110"/>
-      <c r="U6" s="110"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
-      <c r="Y6" s="110"/>
-      <c r="Z6" s="110"/>
-      <c r="AA6" s="110"/>
-      <c r="AB6" s="110"/>
-      <c r="AC6" s="110"/>
-      <c r="AD6" s="110"/>
-      <c r="AE6" s="111"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="149"/>
+      <c r="AB6" s="149"/>
+      <c r="AC6" s="149"/>
+      <c r="AD6" s="149"/>
+      <c r="AE6" s="150"/>
     </row>
     <row r="7" spans="1:32" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="151" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="117"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="153"/>
       <c r="E7" s="30"/>
       <c r="F7" s="31" t="s">
         <v>13</v>
@@ -2270,11 +2272,11 @@
       <c r="A8" s="34">
         <v>1</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="143"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="132"/>
       <c r="E8" s="4"/>
       <c r="F8" s="58">
         <v>30</v>
@@ -2320,11 +2322,11 @@
       <c r="A9" s="35">
         <v>2</v>
       </c>
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="114"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="111"/>
       <c r="E9" s="4"/>
       <c r="F9" s="58">
         <v>5</v>
@@ -2366,11 +2368,11 @@
       <c r="A10" s="35">
         <v>3</v>
       </c>
-      <c r="B10" s="120" t="s">
+      <c r="B10" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="114"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="111"/>
       <c r="E10" s="4"/>
       <c r="F10" s="58">
         <v>15</v>
@@ -2414,11 +2416,11 @@
       <c r="A11" s="36">
         <v>4</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="141" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="112"/>
-      <c r="D11" s="119"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="106"/>
       <c r="E11" s="4"/>
       <c r="F11" s="58">
         <v>80</v>
@@ -2515,11 +2517,11 @@
       <c r="A13" s="97">
         <v>6</v>
       </c>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="119"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="106"/>
       <c r="E13" s="4"/>
       <c r="F13" s="58">
         <v>70</v>
@@ -2563,11 +2565,11 @@
       <c r="A14" s="97">
         <v>7</v>
       </c>
-      <c r="B14" s="112" t="s">
+      <c r="B14" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="112"/>
-      <c r="D14" s="119"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="106"/>
       <c r="E14" s="4"/>
       <c r="F14" s="58">
         <v>30</v>
@@ -2611,11 +2613,11 @@
       <c r="A15" s="97">
         <v>8</v>
       </c>
-      <c r="B15" s="112" t="s">
+      <c r="B15" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="112"/>
-      <c r="D15" s="119"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
       <c r="E15" s="4"/>
       <c r="F15" s="58">
         <v>70</v>
@@ -2659,11 +2661,11 @@
       <c r="A16" s="97">
         <v>9</v>
       </c>
-      <c r="B16" s="112" t="s">
+      <c r="B16" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="119"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="106"/>
       <c r="E16" s="4"/>
       <c r="F16" s="58">
         <v>40</v>
@@ -2707,11 +2709,11 @@
       <c r="A17" s="97">
         <v>10</v>
       </c>
-      <c r="B17" s="112" t="s">
+      <c r="B17" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="112"/>
-      <c r="D17" s="119"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="106"/>
       <c r="E17" s="4"/>
       <c r="F17" s="58">
         <v>80</v>
@@ -2807,11 +2809,11 @@
       <c r="A19" s="97">
         <v>12</v>
       </c>
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="114"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="111"/>
       <c r="E19" s="4"/>
       <c r="F19" s="58">
         <v>50</v>
@@ -2855,11 +2857,11 @@
       <c r="A20" s="97">
         <v>13</v>
       </c>
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="141" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="119"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="106"/>
       <c r="E20" s="4"/>
       <c r="F20" s="58">
         <v>20</v>
@@ -2901,11 +2903,11 @@
       <c r="A21" s="97">
         <v>14</v>
       </c>
-      <c r="B21" s="118" t="s">
+      <c r="B21" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="119"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="106"/>
       <c r="E21" s="4"/>
       <c r="F21" s="58">
         <v>100</v>
@@ -2959,11 +2961,11 @@
       <c r="A22" s="97">
         <v>15</v>
       </c>
-      <c r="B22" s="112" t="s">
+      <c r="B22" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="112"/>
-      <c r="D22" s="119"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="106"/>
       <c r="E22" s="4"/>
       <c r="F22" s="58">
         <v>100</v>
@@ -3009,11 +3011,11 @@
       <c r="A23" s="97">
         <v>16</v>
       </c>
-      <c r="B23" s="112" t="s">
+      <c r="B23" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="112"/>
-      <c r="D23" s="119"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="106"/>
       <c r="E23" s="4"/>
       <c r="F23" s="57">
         <v>20</v>
@@ -3055,11 +3057,11 @@
       <c r="A24" s="97">
         <v>17</v>
       </c>
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="112"/>
-      <c r="D24" s="119"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="106"/>
       <c r="E24" s="7"/>
       <c r="F24" s="58">
         <v>100</v>
@@ -3113,11 +3115,11 @@
       <c r="A25" s="98">
         <v>18</v>
       </c>
-      <c r="B25" s="112" t="s">
+      <c r="B25" s="105" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="119"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="106"/>
       <c r="E25" s="4"/>
       <c r="F25" s="8">
         <v>100</v>
@@ -3160,11 +3162,11 @@
       <c r="A26" s="98">
         <v>19</v>
       </c>
-      <c r="B26" s="156" t="s">
+      <c r="B26" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="156"/>
-      <c r="D26" s="156"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
       <c r="E26" s="4"/>
       <c r="F26" s="57">
         <v>200</v>
@@ -3204,11 +3206,11 @@
       <c r="A27" s="97">
         <v>20</v>
       </c>
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
       <c r="E27" s="4"/>
       <c r="F27" s="8">
         <v>50</v>
@@ -3262,11 +3264,11 @@
       <c r="A28" s="97">
         <v>21</v>
       </c>
-      <c r="B28" s="156" t="s">
+      <c r="B28" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="104"/>
       <c r="E28" s="4"/>
       <c r="F28" s="8">
         <v>50</v>
@@ -3368,11 +3370,11 @@
       <c r="A30" s="97">
         <v>23</v>
       </c>
-      <c r="B30" s="156" t="s">
+      <c r="B30" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="156"/>
-      <c r="D30" s="156"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="104"/>
       <c r="E30" s="4"/>
       <c r="F30" s="8">
         <v>25</v>
@@ -3418,11 +3420,11 @@
       <c r="A31" s="97">
         <v>24</v>
       </c>
-      <c r="B31" s="156" t="s">
+      <c r="B31" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="156"/>
-      <c r="D31" s="156"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
       <c r="E31" s="4"/>
       <c r="F31" s="8">
         <v>25</v>
@@ -3468,11 +3470,11 @@
       <c r="A32" s="97">
         <v>25</v>
       </c>
-      <c r="B32" s="156" t="s">
+      <c r="B32" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="156"/>
-      <c r="D32" s="156"/>
+      <c r="C32" s="104"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="4"/>
       <c r="F32" s="8">
         <v>10</v>
@@ -3516,11 +3518,11 @@
       <c r="A33" s="97">
         <v>26</v>
       </c>
-      <c r="B33" s="156" t="s">
+      <c r="B33" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="156"/>
-      <c r="D33" s="156"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="104"/>
       <c r="E33" s="4"/>
       <c r="F33" s="8">
         <v>10</v>
@@ -3600,16 +3602,16 @@
       <c r="A35" s="97">
         <v>28</v>
       </c>
-      <c r="B35" s="156" t="s">
+      <c r="B35" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="157"/>
-      <c r="D35" s="157"/>
+      <c r="C35" s="109"/>
+      <c r="D35" s="109"/>
       <c r="E35" s="4"/>
       <c r="F35" s="8">
         <v>40</v>
       </c>
-      <c r="G35" s="65" t="s">
+      <c r="G35" s="194" t="s">
         <v>57</v>
       </c>
       <c r="H35" s="59"/>
@@ -3674,9 +3676,9 @@
       <c r="A36" s="97">
         <v>29</v>
       </c>
-      <c r="B36" s="139"/>
-      <c r="C36" s="139"/>
-      <c r="D36" s="140"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="107"/>
+      <c r="D36" s="108"/>
       <c r="E36" s="4"/>
       <c r="F36" s="58"/>
       <c r="G36" s="5"/>
@@ -3712,11 +3714,11 @@
       <c r="A37" s="97">
         <v>30</v>
       </c>
-      <c r="B37" s="112" t="s">
+      <c r="B37" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="113"/>
-      <c r="D37" s="114"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="111"/>
       <c r="E37" s="4"/>
       <c r="F37" s="58"/>
       <c r="G37" s="5"/>
@@ -3754,11 +3756,11 @@
       <c r="A38" s="97">
         <v>31</v>
       </c>
-      <c r="B38" s="154" t="s">
+      <c r="B38" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="155"/>
-      <c r="D38" s="155"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="113"/>
       <c r="E38" s="4"/>
       <c r="F38" s="58"/>
       <c r="G38" s="5"/>
@@ -3796,11 +3798,11 @@
       <c r="A39" s="97">
         <v>32</v>
       </c>
-      <c r="B39" s="112" t="s">
+      <c r="B39" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="113"/>
-      <c r="D39" s="114"/>
+      <c r="C39" s="110"/>
+      <c r="D39" s="111"/>
       <c r="E39" s="12"/>
       <c r="F39" s="9"/>
       <c r="G39" s="5"/>
@@ -3838,11 +3840,11 @@
       <c r="A40" s="97">
         <v>33</v>
       </c>
-      <c r="B40" s="154" t="s">
+      <c r="B40" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="155"/>
-      <c r="D40" s="155"/>
+      <c r="C40" s="113"/>
+      <c r="D40" s="113"/>
       <c r="E40" s="4"/>
       <c r="F40" s="58"/>
       <c r="G40" s="5"/>
@@ -3879,11 +3881,11 @@
       <c r="A41" s="97">
         <v>34</v>
       </c>
-      <c r="B41" s="112" t="s">
+      <c r="B41" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="114"/>
+      <c r="C41" s="110"/>
+      <c r="D41" s="111"/>
       <c r="E41" s="4"/>
       <c r="F41" s="63"/>
       <c r="G41" s="5"/>
@@ -3919,11 +3921,11 @@
       <c r="A42" s="97">
         <v>35</v>
       </c>
-      <c r="B42" s="154" t="s">
+      <c r="B42" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="155"/>
-      <c r="D42" s="155"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="113"/>
       <c r="E42" s="4"/>
       <c r="F42" s="58"/>
       <c r="G42" s="14"/>
@@ -3961,11 +3963,11 @@
       <c r="A43" s="97">
         <v>36</v>
       </c>
-      <c r="B43" s="112" t="s">
+      <c r="B43" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="113"/>
-      <c r="D43" s="114"/>
+      <c r="C43" s="110"/>
+      <c r="D43" s="111"/>
       <c r="E43" s="4"/>
       <c r="F43" s="9"/>
       <c r="G43" s="73"/>
@@ -4003,9 +4005,9 @@
       <c r="A44" s="97">
         <v>37</v>
       </c>
-      <c r="B44" s="139"/>
-      <c r="C44" s="139"/>
-      <c r="D44" s="140"/>
+      <c r="B44" s="107"/>
+      <c r="C44" s="107"/>
+      <c r="D44" s="108"/>
       <c r="E44" s="4"/>
       <c r="F44" s="58"/>
       <c r="G44" s="73"/>
@@ -4041,11 +4043,11 @@
       <c r="A45" s="97">
         <v>38</v>
       </c>
-      <c r="B45" s="112" t="s">
+      <c r="B45" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="113"/>
-      <c r="D45" s="114"/>
+      <c r="C45" s="110"/>
+      <c r="D45" s="111"/>
       <c r="E45" s="4"/>
       <c r="F45" s="63"/>
       <c r="G45" s="73"/>
@@ -4081,11 +4083,11 @@
       <c r="A46" s="97">
         <v>39</v>
       </c>
-      <c r="B46" s="112" t="s">
+      <c r="B46" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="113"/>
-      <c r="D46" s="114"/>
+      <c r="C46" s="110"/>
+      <c r="D46" s="111"/>
       <c r="E46" s="4"/>
       <c r="F46" s="58"/>
       <c r="G46" s="73"/>
@@ -4121,11 +4123,11 @@
       <c r="A47" s="97">
         <v>40</v>
       </c>
-      <c r="B47" s="112" t="s">
+      <c r="B47" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="113"/>
-      <c r="D47" s="114"/>
+      <c r="C47" s="110"/>
+      <c r="D47" s="111"/>
       <c r="E47" s="4"/>
       <c r="F47" s="9"/>
       <c r="G47" s="73"/>
@@ -4161,11 +4163,11 @@
       <c r="A48" s="97">
         <v>41</v>
       </c>
-      <c r="B48" s="112" t="s">
+      <c r="B48" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="113"/>
-      <c r="D48" s="114"/>
+      <c r="C48" s="110"/>
+      <c r="D48" s="111"/>
       <c r="E48" s="4"/>
       <c r="F48" s="58"/>
       <c r="G48" s="73"/>
@@ -4201,11 +4203,11 @@
       <c r="A49" s="97">
         <v>42</v>
       </c>
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="114"/>
+      <c r="C49" s="110"/>
+      <c r="D49" s="111"/>
       <c r="E49" s="4"/>
       <c r="F49" s="58"/>
       <c r="G49" s="73"/>
@@ -4241,11 +4243,11 @@
       <c r="A50" s="97">
         <v>43</v>
       </c>
-      <c r="B50" s="112" t="s">
+      <c r="B50" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="113"/>
-      <c r="D50" s="114"/>
+      <c r="C50" s="110"/>
+      <c r="D50" s="111"/>
       <c r="E50" s="4"/>
       <c r="F50" s="9"/>
       <c r="G50" s="73"/>
@@ -4281,11 +4283,11 @@
       <c r="A51" s="97">
         <v>44</v>
       </c>
-      <c r="B51" s="112" t="s">
+      <c r="B51" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="113"/>
-      <c r="D51" s="114"/>
+      <c r="C51" s="110"/>
+      <c r="D51" s="111"/>
       <c r="E51" s="4"/>
       <c r="F51" s="58"/>
       <c r="G51" s="73"/>
@@ -4321,11 +4323,11 @@
       <c r="A52" s="97">
         <v>45</v>
       </c>
-      <c r="B52" s="112" t="s">
+      <c r="B52" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="113"/>
-      <c r="D52" s="114"/>
+      <c r="C52" s="110"/>
+      <c r="D52" s="111"/>
       <c r="E52" s="4"/>
       <c r="F52" s="63"/>
       <c r="G52" s="73"/>
@@ -4361,11 +4363,11 @@
       <c r="A53" s="97">
         <v>46</v>
       </c>
-      <c r="B53" s="112" t="s">
+      <c r="B53" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="113"/>
-      <c r="D53" s="114"/>
+      <c r="C53" s="110"/>
+      <c r="D53" s="111"/>
       <c r="E53" s="4"/>
       <c r="F53" s="58"/>
       <c r="G53" s="73"/>
@@ -4401,11 +4403,11 @@
       <c r="A54" s="97">
         <v>47</v>
       </c>
-      <c r="B54" s="112" t="s">
+      <c r="B54" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="113"/>
-      <c r="D54" s="114"/>
+      <c r="C54" s="110"/>
+      <c r="D54" s="111"/>
       <c r="E54" s="4"/>
       <c r="F54" s="9"/>
       <c r="G54" s="73"/>
@@ -4440,11 +4442,11 @@
       <c r="A55" s="97">
         <v>48</v>
       </c>
-      <c r="B55" s="112" t="s">
+      <c r="B55" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="113"/>
-      <c r="D55" s="114"/>
+      <c r="C55" s="110"/>
+      <c r="D55" s="111"/>
       <c r="E55" s="4"/>
       <c r="F55" s="58"/>
       <c r="G55" s="73"/>
@@ -4480,11 +4482,11 @@
       <c r="A56" s="97">
         <v>49</v>
       </c>
-      <c r="B56" s="112" t="s">
+      <c r="B56" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="113"/>
-      <c r="D56" s="114"/>
+      <c r="C56" s="110"/>
+      <c r="D56" s="111"/>
       <c r="E56" s="4"/>
       <c r="F56" s="63"/>
       <c r="G56" s="73"/>
@@ -4519,9 +4521,9 @@
       <c r="A57" s="97">
         <v>50</v>
       </c>
-      <c r="B57" s="152"/>
-      <c r="C57" s="152"/>
-      <c r="D57" s="153"/>
+      <c r="B57" s="114"/>
+      <c r="C57" s="114"/>
+      <c r="D57" s="115"/>
       <c r="E57" s="4"/>
       <c r="F57" s="58"/>
       <c r="G57" s="74"/>
@@ -4557,9 +4559,9 @@
       <c r="A58" s="98">
         <v>51</v>
       </c>
-      <c r="B58" s="152"/>
-      <c r="C58" s="152"/>
-      <c r="D58" s="153"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="114"/>
+      <c r="D58" s="115"/>
       <c r="E58" s="4"/>
       <c r="F58" s="11"/>
       <c r="G58" s="12"/>
@@ -4593,11 +4595,11 @@
     </row>
     <row r="59" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="96"/>
-      <c r="B59" s="127" t="s">
+      <c r="B59" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="C59" s="127"/>
-      <c r="D59" s="128"/>
+      <c r="C59" s="133"/>
+      <c r="D59" s="134"/>
       <c r="E59" s="39"/>
       <c r="F59" s="40">
         <f>SUM(F8:F43)</f>
@@ -4775,41 +4777,23 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="70">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="U3:AE3"/>
-    <mergeCell ref="P5:AE5"/>
-    <mergeCell ref="Q4:AD4"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="D2:AE2"/>
+    <mergeCell ref="H6:AE6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
@@ -4826,25 +4810,43 @@
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B24:D24"/>
+    <mergeCell ref="U3:AE3"/>
+    <mergeCell ref="P5:AE5"/>
+    <mergeCell ref="Q4:AD4"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B51:D51"/>
     <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="D2:AE2"/>
-    <mergeCell ref="H6:AE6"/>
     <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -4860,8 +4862,8 @@
   </sheetPr>
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4876,240 +4878,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="175" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="164"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="176"/>
+      <c r="U1" s="176"/>
+      <c r="V1" s="176"/>
+      <c r="W1" s="176"/>
+      <c r="X1" s="176"/>
+      <c r="Y1" s="176"/>
+      <c r="Z1" s="176"/>
+      <c r="AA1" s="176"/>
+      <c r="AB1" s="176"/>
+      <c r="AC1" s="176"/>
+      <c r="AD1" s="177"/>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="168"/>
+      <c r="B2" s="181"/>
       <c r="C2" s="45"/>
-      <c r="D2" s="165" t="str">
+      <c r="D2" s="178" t="str">
         <f>Basplan!D2</f>
         <v>Undsättningsrobot</v>
       </c>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="165"/>
-      <c r="P2" s="165"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="165"/>
-      <c r="S2" s="165"/>
-      <c r="T2" s="165"/>
-      <c r="U2" s="165"/>
-      <c r="V2" s="165"/>
-      <c r="W2" s="165"/>
-      <c r="X2" s="165"/>
-      <c r="Y2" s="165"/>
-      <c r="Z2" s="165"/>
-      <c r="AA2" s="165"/>
-      <c r="AB2" s="165"/>
-      <c r="AC2" s="165"/>
-      <c r="AD2" s="166"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
+      <c r="Q2" s="178"/>
+      <c r="R2" s="178"/>
+      <c r="S2" s="178"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="178"/>
+      <c r="V2" s="178"/>
+      <c r="W2" s="178"/>
+      <c r="X2" s="178"/>
+      <c r="Y2" s="178"/>
+      <c r="Z2" s="178"/>
+      <c r="AA2" s="178"/>
+      <c r="AB2" s="178"/>
+      <c r="AC2" s="178"/>
+      <c r="AD2" s="179"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="182" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="170"/>
+      <c r="B3" s="183"/>
       <c r="C3" s="46"/>
-      <c r="D3" s="171">
+      <c r="D3" s="184">
         <f>Basplan!D3</f>
         <v>2</v>
       </c>
-      <c r="E3" s="172"/>
-      <c r="F3" s="172"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="137" t="s">
+      <c r="E3" s="185"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="174"/>
-      <c r="L3" s="121">
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="154">
         <v>42051</v>
       </c>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="176"/>
+      <c r="M3" s="188"/>
+      <c r="N3" s="188"/>
+      <c r="O3" s="188"/>
+      <c r="P3" s="188"/>
+      <c r="Q3" s="188"/>
+      <c r="R3" s="188"/>
+      <c r="S3" s="188"/>
+      <c r="T3" s="188"/>
+      <c r="U3" s="188"/>
+      <c r="V3" s="188"/>
+      <c r="W3" s="188"/>
+      <c r="X3" s="188"/>
+      <c r="Y3" s="188"/>
+      <c r="Z3" s="188"/>
+      <c r="AA3" s="188"/>
+      <c r="AB3" s="188"/>
+      <c r="AC3" s="188"/>
+      <c r="AD3" s="189"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="188"/>
+      <c r="A4" s="159" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="169"/>
       <c r="C4" s="47"/>
-      <c r="D4" s="189" t="str">
+      <c r="D4" s="170" t="str">
         <f>Basplan!D4</f>
         <v>Kent Palmkvist</v>
       </c>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="191"/>
-      <c r="H4" s="178" t="s">
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="159" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="179"/>
-      <c r="J4" s="179"/>
-      <c r="K4" s="179"/>
-      <c r="L4" s="180" t="s">
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
+      <c r="L4" s="161" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="181"/>
-      <c r="N4" s="181"/>
-      <c r="O4" s="181"/>
-      <c r="P4" s="181"/>
-      <c r="Q4" s="181"/>
-      <c r="R4" s="181"/>
-      <c r="S4" s="181"/>
-      <c r="T4" s="181"/>
-      <c r="U4" s="181"/>
-      <c r="V4" s="181"/>
-      <c r="W4" s="181"/>
-      <c r="X4" s="181"/>
-      <c r="Y4" s="181"/>
-      <c r="Z4" s="181"/>
-      <c r="AA4" s="181"/>
-      <c r="AB4" s="181"/>
-      <c r="AC4" s="181"/>
-      <c r="AD4" s="182"/>
+      <c r="M4" s="162"/>
+      <c r="N4" s="162"/>
+      <c r="O4" s="162"/>
+      <c r="P4" s="162"/>
+      <c r="Q4" s="162"/>
+      <c r="R4" s="162"/>
+      <c r="S4" s="162"/>
+      <c r="T4" s="162"/>
+      <c r="U4" s="162"/>
+      <c r="V4" s="162"/>
+      <c r="W4" s="162"/>
+      <c r="X4" s="162"/>
+      <c r="Y4" s="162"/>
+      <c r="Z4" s="162"/>
+      <c r="AA4" s="162"/>
+      <c r="AB4" s="162"/>
+      <c r="AC4" s="162"/>
+      <c r="AD4" s="163"/>
     </row>
     <row r="5" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="192" t="s">
+      <c r="A5" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="193"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="48"/>
-      <c r="D5" s="159" t="str">
+      <c r="D5" s="190" t="str">
         <f>Basplan!D5</f>
         <v>TSEA56</v>
       </c>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="148"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="158"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="119"/>
+      <c r="M5" s="119"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="119"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119"/>
+      <c r="T5" s="119"/>
+      <c r="U5" s="119"/>
+      <c r="V5" s="119"/>
+      <c r="W5" s="119"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="119"/>
+      <c r="Z5" s="119"/>
+      <c r="AA5" s="119"/>
+      <c r="AB5" s="119"/>
+      <c r="AC5" s="119"/>
+      <c r="AD5" s="120"/>
     </row>
     <row r="6" spans="1:31" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="186" t="s">
+      <c r="A6" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="187"/>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="183" t="s">
+      <c r="B6" s="168"/>
+      <c r="C6" s="168"/>
+      <c r="D6" s="168"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184"/>
-      <c r="J6" s="184"/>
-      <c r="K6" s="184"/>
-      <c r="L6" s="184"/>
-      <c r="M6" s="184"/>
-      <c r="N6" s="184"/>
-      <c r="O6" s="184"/>
-      <c r="P6" s="184"/>
-      <c r="Q6" s="184"/>
-      <c r="R6" s="184"/>
-      <c r="S6" s="184"/>
-      <c r="T6" s="184"/>
-      <c r="U6" s="184"/>
-      <c r="V6" s="184"/>
-      <c r="W6" s="184"/>
-      <c r="X6" s="184"/>
-      <c r="Y6" s="184"/>
-      <c r="Z6" s="184"/>
-      <c r="AA6" s="184"/>
-      <c r="AB6" s="184"/>
-      <c r="AC6" s="184"/>
-      <c r="AD6" s="185"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="165"/>
+      <c r="L6" s="165"/>
+      <c r="M6" s="165"/>
+      <c r="N6" s="165"/>
+      <c r="O6" s="165"/>
+      <c r="P6" s="165"/>
+      <c r="Q6" s="165"/>
+      <c r="R6" s="165"/>
+      <c r="S6" s="165"/>
+      <c r="T6" s="165"/>
+      <c r="U6" s="165"/>
+      <c r="V6" s="165"/>
+      <c r="W6" s="165"/>
+      <c r="X6" s="165"/>
+      <c r="Y6" s="165"/>
+      <c r="Z6" s="165"/>
+      <c r="AA6" s="165"/>
+      <c r="AB6" s="165"/>
+      <c r="AC6" s="165"/>
+      <c r="AD6" s="166"/>
     </row>
     <row r="7" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
       <c r="G7" s="31">
         <f>Basplan!H7</f>
         <v>1</v>
@@ -5208,13 +5210,13 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="143"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
       <c r="G8" s="66"/>
       <c r="H8" s="67"/>
       <c r="I8" s="67"/>
@@ -5251,13 +5253,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="114"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="111"/>
       <c r="G9" s="68"/>
       <c r="H9" s="69"/>
       <c r="I9" s="69"/>
@@ -5294,13 +5296,13 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
-      <c r="B10" s="120" t="s">
+      <c r="B10" s="142" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="111"/>
       <c r="G10" s="68"/>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
@@ -5337,13 +5339,13 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="114"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="111"/>
       <c r="G11" s="68"/>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
@@ -5380,13 +5382,13 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="54"/>
-      <c r="B12" s="120" t="s">
+      <c r="B12" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="114"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="111"/>
       <c r="G12" s="68"/>
       <c r="H12" s="69"/>
       <c r="I12" s="69"/>
@@ -5424,13 +5426,13 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
-      <c r="B13" s="120" t="s">
+      <c r="B13" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
       <c r="G13" s="68"/>
       <c r="H13" s="69"/>
       <c r="I13" s="69"/>
@@ -5467,11 +5469,11 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
-      <c r="B14" s="120"/>
-      <c r="C14" s="113"/>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
+      <c r="B14" s="142"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
       <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -5502,11 +5504,11 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
-      <c r="B15" s="120"/>
-      <c r="C15" s="113"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
+      <c r="B15" s="142"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="110"/>
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
@@ -5537,11 +5539,11 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
-      <c r="B16" s="120"/>
-      <c r="C16" s="113"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="113"/>
+      <c r="B16" s="142"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -5572,11 +5574,11 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
+      <c r="B17" s="142"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -5607,11 +5609,11 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="113"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -5642,11 +5644,11 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
-      <c r="B19" s="120"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
@@ -5677,11 +5679,11 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
-      <c r="B20" s="120"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="113"/>
+      <c r="B20" s="142"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
       <c r="G20" s="18"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -5712,11 +5714,11 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
+      <c r="B21" s="142"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="110"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -5747,11 +5749,11 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="113"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="113"/>
+      <c r="B22" s="142"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
@@ -5782,11 +5784,11 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="54"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
       <c r="G23" s="18"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -5817,11 +5819,11 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="54"/>
-      <c r="B24" s="120"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
+      <c r="B24" s="142"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
       <c r="G24" s="18"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
@@ -5852,11 +5854,11 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
       <c r="G25" s="18"/>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
@@ -5887,11 +5889,11 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
+      <c r="B26" s="142"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
       <c r="G26" s="18"/>
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
@@ -5922,11 +5924,11 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
-      <c r="B27" s="120"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113"/>
+      <c r="B27" s="142"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
       <c r="G27" s="18"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
@@ -5957,11 +5959,11 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="55"/>
-      <c r="B28" s="120"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="113"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
       <c r="G28" s="18"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
@@ -5992,11 +5994,11 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="55"/>
-      <c r="B29" s="120"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="113"/>
+      <c r="B29" s="142"/>
+      <c r="C29" s="110"/>
+      <c r="D29" s="110"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="110"/>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
@@ -6027,11 +6029,11 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="54"/>
-      <c r="B30" s="120"/>
-      <c r="C30" s="113"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="113"/>
-      <c r="F30" s="113"/>
+      <c r="B30" s="142"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
       <c r="G30" s="18"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
@@ -6062,11 +6064,11 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="54"/>
-      <c r="B31" s="120"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="110"/>
+      <c r="D31" s="110"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="110"/>
       <c r="G31" s="18"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
@@ -6097,11 +6099,11 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="54"/>
-      <c r="B32" s="120"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="113"/>
-      <c r="F32" s="113"/>
+      <c r="B32" s="142"/>
+      <c r="C32" s="110"/>
+      <c r="D32" s="110"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="110"/>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
@@ -6132,11 +6134,11 @@
     </row>
     <row r="33" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="54"/>
-      <c r="B33" s="158"/>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
+      <c r="B33" s="193"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="114"/>
       <c r="G33" s="21"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -6167,13 +6169,13 @@
     </row>
     <row r="34" spans="1:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
-      <c r="B34" s="127" t="s">
+      <c r="B34" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="127"/>
-      <c r="D34" s="127"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
+      <c r="C34" s="133"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="133"/>
       <c r="G34" s="56">
         <f>SUM(G8:G33)</f>
         <v>0</v>
@@ -6274,6 +6276,34 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="D2:AD2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:AD3"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="H5:AD5"/>
     <mergeCell ref="H4:K4"/>
@@ -6290,34 +6320,6 @@
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="D2:AD2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:AD3"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.71" top="1" bottom="1" header="0.5" footer="0.61"/>

</xml_diff>